<commit_message>
fix: inversión inicial $3.500.000 y dividendo $0 en meses de gracia
- Inversión inicial actualizada de $3.200.000 a $3.500.000 CLP
- Dividendo se aplica con IF: $0 durante los 6 meses de gracia,
  $274.000 desde mes 7 en adelante (referencia dinámica a Parámetros)

https://claude.ai/code/session_01Pr8PxEhirEbuLnFTe77xzf
</commit_message>
<xml_diff>
--- a/airbnb/flujo_caja_airbnb.xlsx
+++ b/airbnb/flujo_caja_airbnb.xlsx
@@ -853,7 +853,7 @@
         </is>
       </c>
       <c r="B18" s="6" t="n">
-        <v>3200000</v>
+        <v>3500000</v>
       </c>
     </row>
     <row r="19" ht="20" customHeight="1">
@@ -2594,147 +2594,147 @@
         </is>
       </c>
       <c r="B14" s="21">
-        <f>'Parámetros'!$B$15</f>
+        <f>IF(1&lt;='Parámetros'!$B$5,0,'Parámetros'!$B$15)</f>
         <v/>
       </c>
       <c r="C14" s="21">
-        <f>'Parámetros'!$B$15</f>
+        <f>IF(2&lt;='Parámetros'!$B$5,0,'Parámetros'!$B$15)</f>
         <v/>
       </c>
       <c r="D14" s="21">
-        <f>'Parámetros'!$B$15</f>
+        <f>IF(3&lt;='Parámetros'!$B$5,0,'Parámetros'!$B$15)</f>
         <v/>
       </c>
       <c r="E14" s="21">
-        <f>'Parámetros'!$B$15</f>
+        <f>IF(4&lt;='Parámetros'!$B$5,0,'Parámetros'!$B$15)</f>
         <v/>
       </c>
       <c r="F14" s="21">
-        <f>'Parámetros'!$B$15</f>
+        <f>IF(5&lt;='Parámetros'!$B$5,0,'Parámetros'!$B$15)</f>
         <v/>
       </c>
       <c r="G14" s="21">
-        <f>'Parámetros'!$B$15</f>
+        <f>IF(6&lt;='Parámetros'!$B$5,0,'Parámetros'!$B$15)</f>
         <v/>
       </c>
       <c r="H14" s="21">
-        <f>'Parámetros'!$B$15</f>
+        <f>IF(7&lt;='Parámetros'!$B$5,0,'Parámetros'!$B$15)</f>
         <v/>
       </c>
       <c r="I14" s="21">
-        <f>'Parámetros'!$B$15</f>
+        <f>IF(8&lt;='Parámetros'!$B$5,0,'Parámetros'!$B$15)</f>
         <v/>
       </c>
       <c r="J14" s="21">
-        <f>'Parámetros'!$B$15</f>
+        <f>IF(9&lt;='Parámetros'!$B$5,0,'Parámetros'!$B$15)</f>
         <v/>
       </c>
       <c r="K14" s="21">
-        <f>'Parámetros'!$B$15</f>
+        <f>IF(10&lt;='Parámetros'!$B$5,0,'Parámetros'!$B$15)</f>
         <v/>
       </c>
       <c r="L14" s="21">
-        <f>'Parámetros'!$B$15</f>
+        <f>IF(11&lt;='Parámetros'!$B$5,0,'Parámetros'!$B$15)</f>
         <v/>
       </c>
       <c r="M14" s="21">
-        <f>'Parámetros'!$B$15</f>
+        <f>IF(12&lt;='Parámetros'!$B$5,0,'Parámetros'!$B$15)</f>
         <v/>
       </c>
       <c r="N14" s="21">
-        <f>'Parámetros'!$B$15</f>
+        <f>IF(13&lt;='Parámetros'!$B$5,0,'Parámetros'!$B$15)</f>
         <v/>
       </c>
       <c r="O14" s="21">
-        <f>'Parámetros'!$B$15</f>
+        <f>IF(14&lt;='Parámetros'!$B$5,0,'Parámetros'!$B$15)</f>
         <v/>
       </c>
       <c r="P14" s="21">
-        <f>'Parámetros'!$B$15</f>
+        <f>IF(15&lt;='Parámetros'!$B$5,0,'Parámetros'!$B$15)</f>
         <v/>
       </c>
       <c r="Q14" s="21">
-        <f>'Parámetros'!$B$15</f>
+        <f>IF(16&lt;='Parámetros'!$B$5,0,'Parámetros'!$B$15)</f>
         <v/>
       </c>
       <c r="R14" s="21">
-        <f>'Parámetros'!$B$15</f>
+        <f>IF(17&lt;='Parámetros'!$B$5,0,'Parámetros'!$B$15)</f>
         <v/>
       </c>
       <c r="S14" s="21">
-        <f>'Parámetros'!$B$15</f>
+        <f>IF(18&lt;='Parámetros'!$B$5,0,'Parámetros'!$B$15)</f>
         <v/>
       </c>
       <c r="T14" s="21">
-        <f>'Parámetros'!$B$15</f>
+        <f>IF(19&lt;='Parámetros'!$B$5,0,'Parámetros'!$B$15)</f>
         <v/>
       </c>
       <c r="U14" s="21">
-        <f>'Parámetros'!$B$15</f>
+        <f>IF(20&lt;='Parámetros'!$B$5,0,'Parámetros'!$B$15)</f>
         <v/>
       </c>
       <c r="V14" s="21">
-        <f>'Parámetros'!$B$15</f>
+        <f>IF(21&lt;='Parámetros'!$B$5,0,'Parámetros'!$B$15)</f>
         <v/>
       </c>
       <c r="W14" s="21">
-        <f>'Parámetros'!$B$15</f>
+        <f>IF(22&lt;='Parámetros'!$B$5,0,'Parámetros'!$B$15)</f>
         <v/>
       </c>
       <c r="X14" s="21">
-        <f>'Parámetros'!$B$15</f>
+        <f>IF(23&lt;='Parámetros'!$B$5,0,'Parámetros'!$B$15)</f>
         <v/>
       </c>
       <c r="Y14" s="21">
-        <f>'Parámetros'!$B$15</f>
+        <f>IF(24&lt;='Parámetros'!$B$5,0,'Parámetros'!$B$15)</f>
         <v/>
       </c>
       <c r="Z14" s="21">
-        <f>'Parámetros'!$B$15</f>
+        <f>IF(25&lt;='Parámetros'!$B$5,0,'Parámetros'!$B$15)</f>
         <v/>
       </c>
       <c r="AA14" s="21">
-        <f>'Parámetros'!$B$15</f>
+        <f>IF(26&lt;='Parámetros'!$B$5,0,'Parámetros'!$B$15)</f>
         <v/>
       </c>
       <c r="AB14" s="21">
-        <f>'Parámetros'!$B$15</f>
+        <f>IF(27&lt;='Parámetros'!$B$5,0,'Parámetros'!$B$15)</f>
         <v/>
       </c>
       <c r="AC14" s="21">
-        <f>'Parámetros'!$B$15</f>
+        <f>IF(28&lt;='Parámetros'!$B$5,0,'Parámetros'!$B$15)</f>
         <v/>
       </c>
       <c r="AD14" s="21">
-        <f>'Parámetros'!$B$15</f>
+        <f>IF(29&lt;='Parámetros'!$B$5,0,'Parámetros'!$B$15)</f>
         <v/>
       </c>
       <c r="AE14" s="21">
-        <f>'Parámetros'!$B$15</f>
+        <f>IF(30&lt;='Parámetros'!$B$5,0,'Parámetros'!$B$15)</f>
         <v/>
       </c>
       <c r="AF14" s="21">
-        <f>'Parámetros'!$B$15</f>
+        <f>IF(31&lt;='Parámetros'!$B$5,0,'Parámetros'!$B$15)</f>
         <v/>
       </c>
       <c r="AG14" s="21">
-        <f>'Parámetros'!$B$15</f>
+        <f>IF(32&lt;='Parámetros'!$B$5,0,'Parámetros'!$B$15)</f>
         <v/>
       </c>
       <c r="AH14" s="21">
-        <f>'Parámetros'!$B$15</f>
+        <f>IF(33&lt;='Parámetros'!$B$5,0,'Parámetros'!$B$15)</f>
         <v/>
       </c>
       <c r="AI14" s="21">
-        <f>'Parámetros'!$B$15</f>
+        <f>IF(34&lt;='Parámetros'!$B$5,0,'Parámetros'!$B$15)</f>
         <v/>
       </c>
       <c r="AJ14" s="21">
-        <f>'Parámetros'!$B$15</f>
+        <f>IF(35&lt;='Parámetros'!$B$5,0,'Parámetros'!$B$15)</f>
         <v/>
       </c>
       <c r="AK14" s="21">
-        <f>'Parámetros'!$B$15</f>
+        <f>IF(36&lt;='Parámetros'!$B$5,0,'Parámetros'!$B$15)</f>
         <v/>
       </c>
       <c r="AL14" s="17">

</xml_diff>